<commit_message>
diagrama de Gantt e relatorio (falta rever)
</commit_message>
<xml_diff>
--- a/02Others/DiagramaGantt.xlsx
+++ b/02Others/DiagramaGantt.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\OneDrive\Documentos\MEEIC\3Ano\2Semestre\LPI\DWR-19\02Others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\DWR-19\02Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{242898B0-AD67-4CEF-AFA5-353E30E8ECCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ABEFB9-6053-40D7-9ECC-35310EAD7D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="-120" windowWidth="27840" windowHeight="16440" xr2:uid="{7EAE9B81-44DC-4E8E-B83A-C092215C44BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7EAE9B81-44DC-4E8E-B83A-C092215C44BB}"/>
   </bookViews>
   <sheets>
     <sheet name="1a Versao" sheetId="2" r:id="rId1"/>
+    <sheet name="2a Versao" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t xml:space="preserve">Tarefa </t>
   </si>
@@ -124,6 +125,12 @@
   <si>
     <t>Etapa 1.3: Testes previstos</t>
   </si>
+  <si>
+    <t>Etapa 2.2.2: Algoritmo para a deteção de RFID</t>
+  </si>
+  <si>
+    <t>Etapa 2.2.5: Junção dos módulos e implementação da máquina de estados</t>
+  </si>
 </sst>
 </file>
 
@@ -197,6 +204,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF962118"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -240,8 +252,407 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1a Versao'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Início </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'1a Versao'!$B$3:$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>Etapa 0: Constituição dos grupos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Etapa 0: Seleção de orientador</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Etapa 0: Seleção do projeto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Etapa 0: Estudo da viabilidade </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Etapa 1.1: Descrição do produto</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Etapa 1.2: Especificações previstas</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Etapa 1.3: Testes previstos</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Etapa 1.4: Diagrama de Gantt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Etapa 2: Alterações na maquete</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Etapa 2.1: Estudo e aquisição do material necessário </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Etapa 2.2: Desenho e implementação do seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Etapa 2.2.1: Desenho da estrutura da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etapa 2.2.2: Módulo para acondicionamento de sinal dos sensores</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Etapa 2.2.3: Algoritmo para o seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Etapa 2.2.4: Algoritmo para deteção de obstáculos</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Etapa 2.2.5: Algoritmo para a deteção de RFID</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Etapa 2.2.6: Junção dos módulos e implementação da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Etapa 2.2.7: Teste do módulo</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Etapa 2.3: Desenho e implementação do controlador remoto</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Etapa 2.3.1: Módulo para comunicação sem fios</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Etapa 2.3.2: Criação de uma interface utilizador/controlador</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Etapa 2.3.3: Teste do módulo</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Etapa 2.4: Montagem e validação do produto</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Etapa 2.5: Estudo de Fiabilidade, Certificação e Segurança</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Etapa 2.6: Documentação</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Etapa 2.7: Apresentação</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1a Versao'!$C$3:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44273</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44288</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44288</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44300</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44301</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44301</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44322</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44322</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44338</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44362</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B430-43ED-A434-7D85979961FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1a Versao'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duração</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'1a Versao'!$B$3:$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>Etapa 0: Constituição dos grupos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Etapa 0: Seleção de orientador</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Etapa 0: Seleção do projeto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Etapa 0: Estudo da viabilidade </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Etapa 1.1: Descrição do produto</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Etapa 1.2: Especificações previstas</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Etapa 1.3: Testes previstos</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Etapa 1.4: Diagrama de Gantt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Etapa 2: Alterações na maquete</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Etapa 2.1: Estudo e aquisição do material necessário </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Etapa 2.2: Desenho e implementação do seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Etapa 2.2.1: Desenho da estrutura da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etapa 2.2.2: Módulo para acondicionamento de sinal dos sensores</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Etapa 2.2.3: Algoritmo para o seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Etapa 2.2.4: Algoritmo para deteção de obstáculos</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Etapa 2.2.5: Algoritmo para a deteção de RFID</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Etapa 2.2.6: Junção dos módulos e implementação da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Etapa 2.2.7: Teste do módulo</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Etapa 2.3: Desenho e implementação do controlador remoto</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Etapa 2.3.1: Módulo para comunicação sem fios</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Etapa 2.3.2: Criação de uma interface utilizador/controlador</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Etapa 2.3.3: Teste do módulo</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Etapa 2.4: Montagem e validação do produto</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Etapa 2.5: Estudo de Fiabilidade, Certificação e Segurança</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Etapa 2.6: Documentação</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Etapa 2.7: Apresentação</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1a Versao'!$D$3:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-B430-43ED-A434-7D85979961FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>'1a Versao'!$C$2</c:f>
@@ -436,13 +847,13 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E028-4FDD-9B66-1402ED3208EC}"/>
+              <c16:uniqueId val="{00000002-B430-43ED-A434-7D85979961FA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>'1a Versao'!$D$2</c:f>
@@ -642,7 +1053,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E028-4FDD-9B66-1402ED3208EC}"/>
+              <c16:uniqueId val="{00000004-B430-43ED-A434-7D85979961FA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -797,24 +1208,11 @@
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -844,565 +1242,1962 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.33758073263560473"/>
+          <c:y val="7.407407407407407E-2"/>
+          <c:w val="0.6137812937259659"/>
+          <c:h val="0.8416746864975212"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1a Versao'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Início </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'1a Versao'!$B$3:$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>Etapa 0: Constituição dos grupos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Etapa 0: Seleção de orientador</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Etapa 0: Seleção do projeto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Etapa 0: Estudo da viabilidade </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Etapa 1.1: Descrição do produto</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Etapa 1.2: Especificações previstas</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Etapa 1.3: Testes previstos</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Etapa 1.4: Diagrama de Gantt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Etapa 2: Alterações na maquete</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Etapa 2.1: Estudo e aquisição do material necessário </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Etapa 2.2: Desenho e implementação do seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Etapa 2.2.1: Desenho da estrutura da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etapa 2.2.2: Módulo para acondicionamento de sinal dos sensores</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Etapa 2.2.3: Algoritmo para o seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Etapa 2.2.4: Algoritmo para deteção de obstáculos</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Etapa 2.2.5: Algoritmo para a deteção de RFID</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Etapa 2.2.6: Junção dos módulos e implementação da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Etapa 2.2.7: Teste do módulo</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Etapa 2.3: Desenho e implementação do controlador remoto</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Etapa 2.3.1: Módulo para comunicação sem fios</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Etapa 2.3.2: Criação de uma interface utilizador/controlador</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Etapa 2.3.3: Teste do módulo</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Etapa 2.4: Montagem e validação do produto</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Etapa 2.5: Estudo de Fiabilidade, Certificação e Segurança</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Etapa 2.6: Documentação</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Etapa 2.7: Apresentação</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1a Versao'!$C$3:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44273</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44288</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44288</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44300</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44301</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44301</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44322</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44322</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44338</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44362</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B430-43ED-A434-7D85979961FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1a Versao'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duração</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="962118"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'1a Versao'!$B$3:$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>Etapa 0: Constituição dos grupos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Etapa 0: Seleção de orientador</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Etapa 0: Seleção do projeto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Etapa 0: Estudo da viabilidade </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Etapa 1.1: Descrição do produto</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Etapa 1.2: Especificações previstas</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Etapa 1.3: Testes previstos</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Etapa 1.4: Diagrama de Gantt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Etapa 2: Alterações na maquete</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Etapa 2.1: Estudo e aquisição do material necessário </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Etapa 2.2: Desenho e implementação do seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Etapa 2.2.1: Desenho da estrutura da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etapa 2.2.2: Módulo para acondicionamento de sinal dos sensores</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Etapa 2.2.3: Algoritmo para o seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Etapa 2.2.4: Algoritmo para deteção de obstáculos</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Etapa 2.2.5: Algoritmo para a deteção de RFID</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Etapa 2.2.6: Junção dos módulos e implementação da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Etapa 2.2.7: Teste do módulo</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Etapa 2.3: Desenho e implementação do controlador remoto</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Etapa 2.3.1: Módulo para comunicação sem fios</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Etapa 2.3.2: Criação de uma interface utilizador/controlador</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Etapa 2.3.3: Teste do módulo</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Etapa 2.4: Montagem e validação do produto</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Etapa 2.5: Estudo de Fiabilidade, Certificação e Segurança</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Etapa 2.6: Documentação</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Etapa 2.7: Apresentação</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1a Versao'!$D$3:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-B430-43ED-A434-7D85979961FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1a Versao'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Início </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'1a Versao'!$B$3:$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>Etapa 0: Constituição dos grupos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Etapa 0: Seleção de orientador</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Etapa 0: Seleção do projeto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Etapa 0: Estudo da viabilidade </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Etapa 1.1: Descrição do produto</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Etapa 1.2: Especificações previstas</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Etapa 1.3: Testes previstos</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Etapa 1.4: Diagrama de Gantt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Etapa 2: Alterações na maquete</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Etapa 2.1: Estudo e aquisição do material necessário </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Etapa 2.2: Desenho e implementação do seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Etapa 2.2.1: Desenho da estrutura da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etapa 2.2.2: Módulo para acondicionamento de sinal dos sensores</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Etapa 2.2.3: Algoritmo para o seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Etapa 2.2.4: Algoritmo para deteção de obstáculos</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Etapa 2.2.5: Algoritmo para a deteção de RFID</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Etapa 2.2.6: Junção dos módulos e implementação da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Etapa 2.2.7: Teste do módulo</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Etapa 2.3: Desenho e implementação do controlador remoto</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Etapa 2.3.1: Módulo para comunicação sem fios</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Etapa 2.3.2: Criação de uma interface utilizador/controlador</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Etapa 2.3.3: Teste do módulo</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Etapa 2.4: Montagem e validação do produto</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Etapa 2.5: Estudo de Fiabilidade, Certificação e Segurança</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Etapa 2.6: Documentação</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Etapa 2.7: Apresentação</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1a Versao'!$C$3:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44273</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44288</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44288</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44300</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44301</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44301</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44322</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44322</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>44338</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44362</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B430-43ED-A434-7D85979961FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1a Versao'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duração</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'1a Versao'!$B$3:$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>Etapa 0: Constituição dos grupos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Etapa 0: Seleção de orientador</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Etapa 0: Seleção do projeto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Etapa 0: Estudo da viabilidade </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Etapa 1.1: Descrição do produto</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Etapa 1.2: Especificações previstas</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Etapa 1.3: Testes previstos</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Etapa 1.4: Diagrama de Gantt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Etapa 2: Alterações na maquete</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Etapa 2.1: Estudo e aquisição do material necessário </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Etapa 2.2: Desenho e implementação do seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Etapa 2.2.1: Desenho da estrutura da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etapa 2.2.2: Módulo para acondicionamento de sinal dos sensores</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Etapa 2.2.3: Algoritmo para o seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Etapa 2.2.4: Algoritmo para deteção de obstáculos</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Etapa 2.2.5: Algoritmo para a deteção de RFID</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Etapa 2.2.6: Junção dos módulos e implementação da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Etapa 2.2.7: Teste do módulo</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Etapa 2.3: Desenho e implementação do controlador remoto</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Etapa 2.3.1: Módulo para comunicação sem fios</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Etapa 2.3.2: Criação de uma interface utilizador/controlador</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Etapa 2.3.3: Teste do módulo</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Etapa 2.4: Montagem e validação do produto</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Etapa 2.5: Estudo de Fiabilidade, Certificação e Segurança</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Etapa 2.6: Documentação</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Etapa 2.7: Apresentação</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1a Versao'!$D$3:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B430-43ED-A434-7D85979961FA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="30"/>
+        <c:overlap val="100"/>
+        <c:axId val="1114819488"/>
+        <c:axId val="1468505200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1114819488"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1468505200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1468505200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="44370"/>
+          <c:min val="44246"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1114819488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="7"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.33758073263560473"/>
+          <c:y val="7.407407407407407E-2"/>
+          <c:w val="0.6137812937259659"/>
+          <c:h val="0.8416746864975212"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2a Versao'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Início </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2a Versao'!$B$3:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>Etapa 0: Constituição dos grupos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Etapa 0: Seleção de orientador</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Etapa 0: Seleção do projeto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Etapa 0: Estudo da viabilidade </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Etapa 1.1: Descrição do produto</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Etapa 1.2: Especificações previstas</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Etapa 1.3: Testes previstos</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Etapa 1.4: Diagrama de Gantt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Etapa 2: Alterações na maquete</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Etapa 2.1: Estudo e aquisição do material necessário </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Etapa 2.2: Desenho e implementação do seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Etapa 2.2.1: Desenho da estrutura da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etapa 2.2.2: Algoritmo para a deteção de RFID</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Etapa 2.2.3: Algoritmo para o seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Etapa 2.2.4: Algoritmo para deteção de obstáculos</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Etapa 2.2.5: Junção dos módulos e implementação da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Etapa 2.3.1: Módulo para comunicação sem fios</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Etapa 2.3.2: Criação de uma interface utilizador/controlador</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Etapa 2.4: Montagem e validação do produto</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Etapa 2.5: Estudo de Fiabilidade, Certificação e Segurança</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Etapa 2.6: Documentação</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Etapa 2.7: Apresentação</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2a Versao'!$C$3:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44273</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44340</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44340</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44344</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44352</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44361</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44340</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44338</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44367</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0FC9-444F-9F13-E8C279D0A13D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2a Versao'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duração</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="962118"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2a Versao'!$B$3:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>Etapa 0: Constituição dos grupos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Etapa 0: Seleção de orientador</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Etapa 0: Seleção do projeto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Etapa 0: Estudo da viabilidade </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Etapa 1.1: Descrição do produto</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Etapa 1.2: Especificações previstas</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Etapa 1.3: Testes previstos</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Etapa 1.4: Diagrama de Gantt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Etapa 2: Alterações na maquete</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Etapa 2.1: Estudo e aquisição do material necessário </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Etapa 2.2: Desenho e implementação do seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Etapa 2.2.1: Desenho da estrutura da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etapa 2.2.2: Algoritmo para a deteção de RFID</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Etapa 2.2.3: Algoritmo para o seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Etapa 2.2.4: Algoritmo para deteção de obstáculos</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Etapa 2.2.5: Junção dos módulos e implementação da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Etapa 2.3.1: Módulo para comunicação sem fios</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Etapa 2.3.2: Criação de uma interface utilizador/controlador</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Etapa 2.4: Montagem e validação do produto</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Etapa 2.5: Estudo de Fiabilidade, Certificação e Segurança</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Etapa 2.6: Documentação</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Etapa 2.7: Apresentação</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2a Versao'!$D$3:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0FC9-444F-9F13-E8C279D0A13D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2a Versao'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Início </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2a Versao'!$B$3:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>Etapa 0: Constituição dos grupos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Etapa 0: Seleção de orientador</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Etapa 0: Seleção do projeto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Etapa 0: Estudo da viabilidade </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Etapa 1.1: Descrição do produto</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Etapa 1.2: Especificações previstas</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Etapa 1.3: Testes previstos</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Etapa 1.4: Diagrama de Gantt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Etapa 2: Alterações na maquete</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Etapa 2.1: Estudo e aquisição do material necessário </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Etapa 2.2: Desenho e implementação do seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Etapa 2.2.1: Desenho da estrutura da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etapa 2.2.2: Algoritmo para a deteção de RFID</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Etapa 2.2.3: Algoritmo para o seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Etapa 2.2.4: Algoritmo para deteção de obstáculos</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Etapa 2.2.5: Junção dos módulos e implementação da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Etapa 2.3.1: Módulo para comunicação sem fios</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Etapa 2.3.2: Criação de uma interface utilizador/controlador</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Etapa 2.4: Montagem e validação do produto</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Etapa 2.5: Estudo de Fiabilidade, Certificação e Segurança</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Etapa 2.6: Documentação</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Etapa 2.7: Apresentação</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2a Versao'!$C$3:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>44246</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44247</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44265</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44273</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44281</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44282</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44340</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44340</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44344</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44352</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44361</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>44340</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44338</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44367</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0FC9-444F-9F13-E8C279D0A13D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2a Versao'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duração</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2a Versao'!$B$3:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>Etapa 0: Constituição dos grupos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Etapa 0: Seleção de orientador</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Etapa 0: Seleção do projeto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Etapa 0: Estudo da viabilidade </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Etapa 1.1: Descrição do produto</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Etapa 1.2: Especificações previstas</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Etapa 1.3: Testes previstos</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Etapa 1.4: Diagrama de Gantt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Etapa 2: Alterações na maquete</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Etapa 2.1: Estudo e aquisição do material necessário </c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Etapa 2.2: Desenho e implementação do seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Etapa 2.2.1: Desenho da estrutura da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Etapa 2.2.2: Algoritmo para a deteção de RFID</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Etapa 2.2.3: Algoritmo para o seguidor de linha</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Etapa 2.2.4: Algoritmo para deteção de obstáculos</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Etapa 2.2.5: Junção dos módulos e implementação da máquina de estados</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Etapa 2.3.1: Módulo para comunicação sem fios</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Etapa 2.3.2: Criação de uma interface utilizador/controlador</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Etapa 2.4: Montagem e validação do produto</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Etapa 2.5: Estudo de Fiabilidade, Certificação e Segurança</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Etapa 2.6: Documentação</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Etapa 2.7: Apresentação</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2a Versao'!$D$3:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0FC9-444F-9F13-E8C279D0A13D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="30"/>
+        <c:overlap val="100"/>
+        <c:axId val="1114819488"/>
+        <c:axId val="1468505200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1114819488"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1468505200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1468505200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="44370"/>
+          <c:min val="44246"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1114819488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="7"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76970</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>134697</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>85303</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>71875</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>162273</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>14147</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1410,6 +3205,87 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C12E05A-6A70-4EF2-957E-CE5781A225AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>67349</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>152652</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>177708</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FEEBE79-7ADB-46E3-96C9-44B0DBCAABE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>134696</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>125075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>219999</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>4526</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{929AF9DE-A56C-4B19-B036-E3AEE554CB4E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1731,8 +3607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0838F1F-E677-432B-9109-FD850F2E8F96}">
   <dimension ref="B2:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E28"/>
+    <sheetView zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,4 +4072,415 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F11406E-28E1-49D9-B201-C1E281F70491}">
+  <dimension ref="B2:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P32" sqref="P32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>44246</v>
+      </c>
+      <c r="D3" s="8">
+        <f>E3-C3</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="7">
+        <v>44247</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7">
+        <v>44247</v>
+      </c>
+      <c r="D4" s="8">
+        <f t="shared" ref="D4:D24" si="0">E4-C4</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>44248</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7">
+        <v>44247</v>
+      </c>
+      <c r="D5" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E5" s="7">
+        <v>44254</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7">
+        <v>44247</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E6" s="7">
+        <v>44260</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="7">
+        <v>44261</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E7" s="7">
+        <v>44265</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="7">
+        <v>44265</v>
+      </c>
+      <c r="D8" s="8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E8" s="7">
+        <v>44279</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="7">
+        <v>44265</v>
+      </c>
+      <c r="D9" s="8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E9" s="7">
+        <v>44279</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="7">
+        <v>44273</v>
+      </c>
+      <c r="D10" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E10" s="7">
+        <v>44279</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="7">
+        <v>44281</v>
+      </c>
+      <c r="D11" s="8">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="E11" s="7">
+        <v>44360</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7">
+        <v>44281</v>
+      </c>
+      <c r="D12" s="8">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="E12" s="7">
+        <v>44360</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="7">
+        <v>44282</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="E13" s="7">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="7">
+        <v>44282</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="E14" s="7">
+        <v>44362</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="7">
+        <v>44300</v>
+      </c>
+      <c r="D15" s="8">
+        <f>E15-C15</f>
+        <v>21</v>
+      </c>
+      <c r="E15" s="7">
+        <v>44321</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="7">
+        <v>44340</v>
+      </c>
+      <c r="D16" s="8">
+        <f>E16-C16</f>
+        <v>4</v>
+      </c>
+      <c r="E16" s="7">
+        <v>44344</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="7">
+        <v>44340</v>
+      </c>
+      <c r="D17" s="8">
+        <f>E17-C17</f>
+        <v>4</v>
+      </c>
+      <c r="E17" s="7">
+        <v>44344</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="7">
+        <v>44344</v>
+      </c>
+      <c r="D18" s="8">
+        <f>E18-C18</f>
+        <v>21</v>
+      </c>
+      <c r="E18" s="7">
+        <v>44365</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="7">
+        <v>44352</v>
+      </c>
+      <c r="D19" s="8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E19" s="7">
+        <v>44360</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="7">
+        <v>44361</v>
+      </c>
+      <c r="D20" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E20" s="7">
+        <v>44366</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="7">
+        <v>44340</v>
+      </c>
+      <c r="D21" s="8">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E21" s="7">
+        <v>44369</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="7">
+        <v>44348</v>
+      </c>
+      <c r="D22" s="8">
+        <f>E22-C22</f>
+        <v>20</v>
+      </c>
+      <c r="E22" s="7">
+        <v>44368</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="7">
+        <v>44338</v>
+      </c>
+      <c r="D23" s="8">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E23" s="7">
+        <v>44369</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="7">
+        <v>44367</v>
+      </c>
+      <c r="D24" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E24" s="7">
+        <v>44369</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="6"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+      <c r="E28" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>